<commit_message>
ITC-?? - Update Real Estate Leasing data import mappings, refine XML export structures, adjust row index references, and add new XSD schemas.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaArrendamientoInmuebles.xlsx
+++ b/public/templates/plantillaArrendamientoInmuebles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\isaac\Arrendamiento de inmuebles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1737CC-B591-4B25-9456-0D0FFFA36AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B78EA49-E0C8-4B2D-BE1A-2EA6C6D316C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="9" r:id="rId1"/>
@@ -2793,9 +2793,6 @@
     <t>Domicilio nacional</t>
   </si>
   <si>
-    <t>Datos de contacto del Socio</t>
-  </si>
-  <si>
     <t>Ciudad</t>
   </si>
   <si>
@@ -2977,6 +2974,9 @@
   </si>
   <si>
     <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Datos de contacto</t>
   </si>
 </sst>
 </file>
@@ -3320,10 +3320,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3335,22 +3342,15 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -5428,7 +5428,7 @@
   <dimension ref="A1:BZ104"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="AQ11" sqref="AQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5493,400 +5493,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
+        <v>971</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22" t="s">
+        <v>950</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="28" t="s">
+        <v>951</v>
+      </c>
+      <c r="AQ1" s="28"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="24" t="s">
+        <v>954</v>
+      </c>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="26"/>
+    </row>
+    <row r="2" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>972</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17" t="s">
-        <v>951</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="18" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22" t="s">
+        <v>935</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>940</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22" t="s">
+        <v>912</v>
+      </c>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="29" t="s">
+        <v>944</v>
+      </c>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="22" t="s">
+        <v>914</v>
+      </c>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22" t="s">
+        <v>921</v>
+      </c>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22" t="s">
+        <v>976</v>
+      </c>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22" t="s">
+        <v>909</v>
+      </c>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22" t="s">
+        <v>911</v>
+      </c>
+      <c r="AX2" s="22"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22" t="s">
+        <v>912</v>
+      </c>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="BE2" s="24" t="s">
+        <v>965</v>
+      </c>
+      <c r="BF2" s="25"/>
+      <c r="BG2" s="25"/>
+      <c r="BH2" s="25"/>
+      <c r="BI2" s="25"/>
+      <c r="BJ2" s="25"/>
+      <c r="BK2" s="25"/>
+      <c r="BL2" s="25"/>
+      <c r="BM2" s="25"/>
+      <c r="BN2" s="26"/>
+      <c r="BO2" s="23" t="s">
+        <v>957</v>
+      </c>
+      <c r="BP2" s="23"/>
+      <c r="BQ2" s="23"/>
+      <c r="BR2" s="23"/>
+      <c r="BS2" s="23"/>
+    </row>
+    <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>973</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>974</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>975</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>906</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>937</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>938</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>907</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>910</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>941</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>942</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>943</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>906</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="V3" s="18" t="s">
+        <v>937</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>938</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>907</v>
+      </c>
+      <c r="Z3" s="18" t="s">
+        <v>845</v>
+      </c>
+      <c r="AA3" s="18" t="s">
+        <v>917</v>
+      </c>
+      <c r="AB3" s="18" t="s">
+        <v>918</v>
+      </c>
+      <c r="AC3" s="18" t="s">
+        <v>919</v>
+      </c>
+      <c r="AD3" s="18" t="s">
+        <v>920</v>
+      </c>
+      <c r="AE3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="18" t="s">
+        <v>945</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>915</v>
+      </c>
+      <c r="AH3" s="18" t="s">
+        <v>845</v>
+      </c>
+      <c r="AI3" s="18" t="s">
+        <v>946</v>
+      </c>
+      <c r="AJ3" s="18" t="s">
+        <v>918</v>
+      </c>
+      <c r="AK3" s="18" t="s">
+        <v>919</v>
+      </c>
+      <c r="AL3" s="18" t="s">
+        <v>811</v>
+      </c>
+      <c r="AM3" s="18" t="s">
+        <v>947</v>
+      </c>
+      <c r="AN3" s="18" t="s">
+        <v>948</v>
+      </c>
+      <c r="AO3" s="18" t="s">
+        <v>949</v>
+      </c>
+      <c r="AP3" s="18" t="s">
+        <v>906</v>
+      </c>
+      <c r="AQ3" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="AR3" s="18" t="s">
+        <v>937</v>
+      </c>
+      <c r="AS3" s="18" t="s">
+        <v>938</v>
+      </c>
+      <c r="AT3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="AU3" s="18" t="s">
+        <v>907</v>
+      </c>
+      <c r="AV3" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="AW3" s="18" t="s">
         <v>952</v>
       </c>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="19" t="s">
-        <v>955</v>
-      </c>
-      <c r="BE1" s="20"/>
-      <c r="BF1" s="20"/>
-      <c r="BG1" s="20"/>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-      <c r="BN1" s="20"/>
-      <c r="BO1" s="20"/>
-      <c r="BP1" s="20"/>
-      <c r="BQ1" s="20"/>
-      <c r="BR1" s="20"/>
-      <c r="BS1" s="21"/>
-    </row>
-    <row r="2" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>973</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
-        <v>936</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17" t="s">
+      <c r="AX3" s="18" t="s">
         <v>941</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17" t="s">
-        <v>912</v>
-      </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="22" t="s">
-        <v>945</v>
-      </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="17" t="s">
-        <v>914</v>
-      </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17" t="s">
-        <v>922</v>
-      </c>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="17"/>
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
-      <c r="AL2" s="17"/>
-      <c r="AM2" s="17" t="s">
-        <v>915</v>
-      </c>
-      <c r="AN2" s="17"/>
-      <c r="AO2" s="17"/>
-      <c r="AP2" s="17" t="s">
-        <v>909</v>
-      </c>
-      <c r="AQ2" s="17"/>
-      <c r="AR2" s="17"/>
-      <c r="AS2" s="17"/>
-      <c r="AT2" s="17"/>
-      <c r="AU2" s="17"/>
-      <c r="AV2" s="17"/>
-      <c r="AW2" s="17" t="s">
-        <v>911</v>
-      </c>
-      <c r="AX2" s="17"/>
-      <c r="AY2" s="17"/>
-      <c r="AZ2" s="17"/>
-      <c r="BA2" s="17" t="s">
-        <v>912</v>
-      </c>
-      <c r="BB2" s="17"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="24" t="s">
+      <c r="AY3" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="AZ3" s="18" t="s">
+        <v>939</v>
+      </c>
+      <c r="BA3" s="18" t="s">
+        <v>913</v>
+      </c>
+      <c r="BB3" s="18" t="s">
+        <v>953</v>
+      </c>
+      <c r="BC3" s="19" t="s">
+        <v>943</v>
+      </c>
+      <c r="BD3" s="20" t="s">
         <v>956</v>
       </c>
-      <c r="BE2" s="19" t="s">
+      <c r="BE3" s="20" t="s">
         <v>966</v>
       </c>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="21"/>
-      <c r="BO2" s="25" t="s">
+      <c r="BF3" s="20" t="s">
+        <v>967</v>
+      </c>
+      <c r="BG3" s="20" t="s">
+        <v>968</v>
+      </c>
+      <c r="BH3" s="20" t="s">
+        <v>969</v>
+      </c>
+      <c r="BI3" s="20" t="s">
+        <v>845</v>
+      </c>
+      <c r="BJ3" s="20" t="s">
+        <v>917</v>
+      </c>
+      <c r="BK3" s="20" t="s">
+        <v>918</v>
+      </c>
+      <c r="BL3" s="20" t="s">
+        <v>919</v>
+      </c>
+      <c r="BM3" s="20" t="s">
+        <v>920</v>
+      </c>
+      <c r="BN3" s="20" t="s">
+        <v>970</v>
+      </c>
+      <c r="BO3" s="20" t="s">
         <v>958</v>
       </c>
-      <c r="BP2" s="25"/>
-      <c r="BQ2" s="25"/>
-      <c r="BR2" s="25"/>
-      <c r="BS2" s="25"/>
-    </row>
-    <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>974</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>975</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>976</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>906</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>937</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>938</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>939</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>907</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>910</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>942</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="O3" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="26" t="s">
-        <v>943</v>
-      </c>
-      <c r="R3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="S3" s="26" t="s">
-        <v>944</v>
-      </c>
-      <c r="T3" s="26" t="s">
-        <v>906</v>
-      </c>
-      <c r="U3" s="26" t="s">
-        <v>937</v>
-      </c>
-      <c r="V3" s="26" t="s">
-        <v>938</v>
-      </c>
-      <c r="W3" s="26" t="s">
-        <v>939</v>
-      </c>
-      <c r="X3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="Y3" s="26" t="s">
-        <v>907</v>
-      </c>
-      <c r="Z3" s="26" t="s">
-        <v>845</v>
-      </c>
-      <c r="AA3" s="26" t="s">
-        <v>918</v>
-      </c>
-      <c r="AB3" s="26" t="s">
-        <v>919</v>
-      </c>
-      <c r="AC3" s="26" t="s">
-        <v>920</v>
-      </c>
-      <c r="AD3" s="26" t="s">
-        <v>921</v>
-      </c>
-      <c r="AE3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF3" s="26" t="s">
-        <v>946</v>
-      </c>
-      <c r="AG3" s="26" t="s">
-        <v>916</v>
-      </c>
-      <c r="AH3" s="26" t="s">
-        <v>845</v>
-      </c>
-      <c r="AI3" s="26" t="s">
-        <v>947</v>
-      </c>
-      <c r="AJ3" s="26" t="s">
-        <v>919</v>
-      </c>
-      <c r="AK3" s="26" t="s">
-        <v>920</v>
-      </c>
-      <c r="AL3" s="26" t="s">
-        <v>811</v>
-      </c>
-      <c r="AM3" s="26" t="s">
-        <v>948</v>
-      </c>
-      <c r="AN3" s="26" t="s">
-        <v>949</v>
-      </c>
-      <c r="AO3" s="26" t="s">
-        <v>950</v>
-      </c>
-      <c r="AP3" s="26" t="s">
-        <v>906</v>
-      </c>
-      <c r="AQ3" s="26" t="s">
-        <v>937</v>
-      </c>
-      <c r="AR3" s="26" t="s">
-        <v>938</v>
-      </c>
-      <c r="AS3" s="26" t="s">
-        <v>939</v>
-      </c>
-      <c r="AT3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="AU3" s="26" t="s">
-        <v>907</v>
-      </c>
-      <c r="AV3" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="AW3" s="26" t="s">
-        <v>953</v>
-      </c>
-      <c r="AX3" s="26" t="s">
-        <v>942</v>
-      </c>
-      <c r="AY3" s="26" t="s">
-        <v>908</v>
-      </c>
-      <c r="AZ3" s="26" t="s">
-        <v>940</v>
-      </c>
-      <c r="BA3" s="26" t="s">
-        <v>913</v>
-      </c>
-      <c r="BB3" s="26" t="s">
-        <v>954</v>
-      </c>
-      <c r="BC3" s="27" t="s">
-        <v>944</v>
-      </c>
-      <c r="BD3" s="28" t="s">
-        <v>957</v>
-      </c>
-      <c r="BE3" s="28" t="s">
-        <v>967</v>
-      </c>
-      <c r="BF3" s="28" t="s">
-        <v>968</v>
-      </c>
-      <c r="BG3" s="28" t="s">
-        <v>969</v>
-      </c>
-      <c r="BH3" s="28" t="s">
-        <v>970</v>
-      </c>
-      <c r="BI3" s="28" t="s">
-        <v>845</v>
-      </c>
-      <c r="BJ3" s="28" t="s">
-        <v>918</v>
-      </c>
-      <c r="BK3" s="28" t="s">
-        <v>919</v>
-      </c>
-      <c r="BL3" s="28" t="s">
-        <v>920</v>
-      </c>
-      <c r="BM3" s="28" t="s">
-        <v>921</v>
-      </c>
-      <c r="BN3" s="28" t="s">
-        <v>971</v>
-      </c>
-      <c r="BO3" s="28" t="s">
+      <c r="BP3" s="20" t="s">
+        <v>964</v>
+      </c>
+      <c r="BQ3" s="20" t="s">
         <v>959</v>
       </c>
-      <c r="BP3" s="28" t="s">
-        <v>965</v>
-      </c>
-      <c r="BQ3" s="28" t="s">
+      <c r="BR3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS3" s="20" t="s">
         <v>960</v>
-      </c>
-      <c r="BR3" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="BS3" s="28" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="4" spans="1:71" x14ac:dyDescent="0.25">
@@ -5908,7 +5908,7 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
@@ -5943,11 +5943,11 @@
       <c r="AW4" s="11"/>
       <c r="AX4" s="8"/>
       <c r="AY4" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ4" s="11"/>
       <c r="BA4" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB4" s="11"/>
       <c r="BC4" s="11"/>
@@ -5987,7 +5987,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
@@ -6022,11 +6022,11 @@
       <c r="AW5" s="11"/>
       <c r="AX5" s="8"/>
       <c r="AY5" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ5" s="11"/>
       <c r="BA5" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB5" s="11"/>
       <c r="BC5" s="11"/>
@@ -6066,7 +6066,7 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
@@ -6101,11 +6101,11 @@
       <c r="AW6" s="11"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ6" s="11"/>
       <c r="BA6" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB6" s="11"/>
       <c r="BC6" s="11"/>
@@ -6145,7 +6145,7 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -6180,11 +6180,11 @@
       <c r="AW7" s="11"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ7" s="11"/>
       <c r="BA7" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB7" s="11"/>
       <c r="BC7" s="11"/>
@@ -6209,7 +6209,7 @@
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="29"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
@@ -6224,7 +6224,7 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
@@ -6259,11 +6259,11 @@
       <c r="AW8" s="11"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ8" s="11"/>
       <c r="BA8" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB8" s="11"/>
       <c r="BC8" s="11"/>
@@ -6303,7 +6303,7 @@
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
@@ -6338,11 +6338,11 @@
       <c r="AW9" s="11"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ9" s="11"/>
       <c r="BA9" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB9" s="11"/>
       <c r="BC9" s="11"/>
@@ -6382,7 +6382,7 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
@@ -6417,11 +6417,11 @@
       <c r="AW10" s="11"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ10" s="11"/>
       <c r="BA10" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB10" s="11"/>
       <c r="BC10" s="11"/>
@@ -6461,7 +6461,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
@@ -6496,11 +6496,11 @@
       <c r="AW11" s="11"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ11" s="11"/>
       <c r="BA11" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB11" s="11"/>
       <c r="BC11" s="11"/>
@@ -6540,7 +6540,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
@@ -6575,11 +6575,11 @@
       <c r="AW12" s="11"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ12" s="11"/>
       <c r="BA12" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB12" s="11"/>
       <c r="BC12" s="11"/>
@@ -6619,7 +6619,7 @@
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
@@ -6654,11 +6654,11 @@
       <c r="AW13" s="11"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ13" s="11"/>
       <c r="BA13" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB13" s="11"/>
       <c r="BC13" s="11"/>
@@ -6698,7 +6698,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
@@ -6733,11 +6733,11 @@
       <c r="AW14" s="11"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ14" s="11"/>
       <c r="BA14" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB14" s="11"/>
       <c r="BC14" s="11"/>
@@ -6777,7 +6777,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
@@ -6812,11 +6812,11 @@
       <c r="AW15" s="11"/>
       <c r="AX15" s="8"/>
       <c r="AY15" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ15" s="11"/>
       <c r="BA15" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB15" s="11"/>
       <c r="BC15" s="11"/>
@@ -6856,7 +6856,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
@@ -6891,11 +6891,11 @@
       <c r="AW16" s="11"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ16" s="11"/>
       <c r="BA16" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB16" s="11"/>
       <c r="BC16" s="11"/>
@@ -6935,7 +6935,7 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
@@ -6970,11 +6970,11 @@
       <c r="AW17" s="11"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ17" s="11"/>
       <c r="BA17" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB17" s="11"/>
       <c r="BC17" s="11"/>
@@ -7014,7 +7014,7 @@
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
@@ -7049,11 +7049,11 @@
       <c r="AW18" s="11"/>
       <c r="AX18" s="8"/>
       <c r="AY18" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ18" s="11"/>
       <c r="BA18" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB18" s="11"/>
       <c r="BC18" s="11"/>
@@ -7093,7 +7093,7 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
@@ -7128,11 +7128,11 @@
       <c r="AW19" s="11"/>
       <c r="AX19" s="8"/>
       <c r="AY19" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ19" s="11"/>
       <c r="BA19" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB19" s="11"/>
       <c r="BC19" s="11"/>
@@ -7172,7 +7172,7 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
@@ -7207,11 +7207,11 @@
       <c r="AW20" s="11"/>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ20" s="11"/>
       <c r="BA20" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB20" s="11"/>
       <c r="BC20" s="11"/>
@@ -7251,7 +7251,7 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
@@ -7286,11 +7286,11 @@
       <c r="AW21" s="11"/>
       <c r="AX21" s="8"/>
       <c r="AY21" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ21" s="11"/>
       <c r="BA21" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB21" s="11"/>
       <c r="BC21" s="11"/>
@@ -7330,7 +7330,7 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
@@ -7365,11 +7365,11 @@
       <c r="AW22" s="11"/>
       <c r="AX22" s="8"/>
       <c r="AY22" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ22" s="11"/>
       <c r="BA22" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB22" s="11"/>
       <c r="BC22" s="11"/>
@@ -7409,7 +7409,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
@@ -7444,11 +7444,11 @@
       <c r="AW23" s="11"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ23" s="11"/>
       <c r="BA23" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB23" s="11"/>
       <c r="BC23" s="11"/>
@@ -7488,7 +7488,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
@@ -7523,11 +7523,11 @@
       <c r="AW24" s="11"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ24" s="11"/>
       <c r="BA24" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB24" s="11"/>
       <c r="BC24" s="11"/>
@@ -7567,7 +7567,7 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
@@ -7602,11 +7602,11 @@
       <c r="AW25" s="11"/>
       <c r="AX25" s="8"/>
       <c r="AY25" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ25" s="11"/>
       <c r="BA25" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB25" s="11"/>
       <c r="BC25" s="11"/>
@@ -7646,7 +7646,7 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
       <c r="R26" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S26" s="11"/>
       <c r="T26" s="11"/>
@@ -7681,11 +7681,11 @@
       <c r="AW26" s="11"/>
       <c r="AX26" s="8"/>
       <c r="AY26" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ26" s="11"/>
       <c r="BA26" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB26" s="11"/>
       <c r="BC26" s="11"/>
@@ -7725,7 +7725,7 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S27" s="11"/>
       <c r="T27" s="11"/>
@@ -7760,11 +7760,11 @@
       <c r="AW27" s="11"/>
       <c r="AX27" s="8"/>
       <c r="AY27" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ27" s="11"/>
       <c r="BA27" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB27" s="11"/>
       <c r="BC27" s="11"/>
@@ -7804,7 +7804,7 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
       <c r="R28" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S28" s="11"/>
       <c r="T28" s="11"/>
@@ -7839,11 +7839,11 @@
       <c r="AW28" s="11"/>
       <c r="AX28" s="8"/>
       <c r="AY28" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ28" s="11"/>
       <c r="BA28" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB28" s="11"/>
       <c r="BC28" s="11"/>
@@ -7883,7 +7883,7 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S29" s="11"/>
       <c r="T29" s="11"/>
@@ -7918,11 +7918,11 @@
       <c r="AW29" s="11"/>
       <c r="AX29" s="8"/>
       <c r="AY29" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ29" s="11"/>
       <c r="BA29" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB29" s="11"/>
       <c r="BC29" s="11"/>
@@ -7962,7 +7962,7 @@
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
       <c r="R30" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S30" s="11"/>
       <c r="T30" s="11"/>
@@ -7997,11 +7997,11 @@
       <c r="AW30" s="11"/>
       <c r="AX30" s="8"/>
       <c r="AY30" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ30" s="11"/>
       <c r="BA30" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB30" s="11"/>
       <c r="BC30" s="11"/>
@@ -8041,7 +8041,7 @@
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
       <c r="R31" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S31" s="11"/>
       <c r="T31" s="11"/>
@@ -8076,11 +8076,11 @@
       <c r="AW31" s="11"/>
       <c r="AX31" s="8"/>
       <c r="AY31" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ31" s="11"/>
       <c r="BA31" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB31" s="11"/>
       <c r="BC31" s="11"/>
@@ -8120,7 +8120,7 @@
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
       <c r="R32" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
@@ -8155,11 +8155,11 @@
       <c r="AW32" s="11"/>
       <c r="AX32" s="8"/>
       <c r="AY32" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ32" s="11"/>
       <c r="BA32" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB32" s="11"/>
       <c r="BC32" s="11"/>
@@ -8199,7 +8199,7 @@
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
       <c r="R33" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S33" s="11"/>
       <c r="T33" s="11"/>
@@ -8234,11 +8234,11 @@
       <c r="AW33" s="11"/>
       <c r="AX33" s="8"/>
       <c r="AY33" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ33" s="11"/>
       <c r="BA33" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB33" s="11"/>
       <c r="BC33" s="11"/>
@@ -8278,7 +8278,7 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
@@ -8313,11 +8313,11 @@
       <c r="AW34" s="11"/>
       <c r="AX34" s="8"/>
       <c r="AY34" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ34" s="11"/>
       <c r="BA34" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB34" s="11"/>
       <c r="BC34" s="11"/>
@@ -8357,7 +8357,7 @@
       <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
       <c r="R35" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
@@ -8392,11 +8392,11 @@
       <c r="AW35" s="11"/>
       <c r="AX35" s="8"/>
       <c r="AY35" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ35" s="11"/>
       <c r="BA35" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB35" s="11"/>
       <c r="BC35" s="11"/>
@@ -8436,7 +8436,7 @@
       <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
       <c r="R36" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>
@@ -8471,11 +8471,11 @@
       <c r="AW36" s="11"/>
       <c r="AX36" s="8"/>
       <c r="AY36" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ36" s="11"/>
       <c r="BA36" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB36" s="11"/>
       <c r="BC36" s="11"/>
@@ -8515,7 +8515,7 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S37" s="11"/>
       <c r="T37" s="11"/>
@@ -8550,11 +8550,11 @@
       <c r="AW37" s="11"/>
       <c r="AX37" s="8"/>
       <c r="AY37" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ37" s="11"/>
       <c r="BA37" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB37" s="11"/>
       <c r="BC37" s="11"/>
@@ -8594,7 +8594,7 @@
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
@@ -8629,11 +8629,11 @@
       <c r="AW38" s="11"/>
       <c r="AX38" s="8"/>
       <c r="AY38" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ38" s="11"/>
       <c r="BA38" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB38" s="11"/>
       <c r="BC38" s="11"/>
@@ -8673,7 +8673,7 @@
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S39" s="11"/>
       <c r="T39" s="11"/>
@@ -8708,11 +8708,11 @@
       <c r="AW39" s="11"/>
       <c r="AX39" s="8"/>
       <c r="AY39" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ39" s="11"/>
       <c r="BA39" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB39" s="11"/>
       <c r="BC39" s="11"/>
@@ -8752,7 +8752,7 @@
       <c r="P40" s="11"/>
       <c r="Q40" s="11"/>
       <c r="R40" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
@@ -8787,11 +8787,11 @@
       <c r="AW40" s="11"/>
       <c r="AX40" s="8"/>
       <c r="AY40" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ40" s="11"/>
       <c r="BA40" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB40" s="11"/>
       <c r="BC40" s="11"/>
@@ -8831,7 +8831,7 @@
       <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
       <c r="R41" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S41" s="11"/>
       <c r="T41" s="11"/>
@@ -8866,11 +8866,11 @@
       <c r="AW41" s="11"/>
       <c r="AX41" s="8"/>
       <c r="AY41" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ41" s="11"/>
       <c r="BA41" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB41" s="11"/>
       <c r="BC41" s="11"/>
@@ -8910,7 +8910,7 @@
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
       <c r="R42" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
@@ -8945,11 +8945,11 @@
       <c r="AW42" s="11"/>
       <c r="AX42" s="8"/>
       <c r="AY42" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ42" s="11"/>
       <c r="BA42" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB42" s="11"/>
       <c r="BC42" s="11"/>
@@ -8989,7 +8989,7 @@
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
       <c r="R43" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S43" s="11"/>
       <c r="T43" s="11"/>
@@ -9024,11 +9024,11 @@
       <c r="AW43" s="11"/>
       <c r="AX43" s="8"/>
       <c r="AY43" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ43" s="11"/>
       <c r="BA43" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB43" s="11"/>
       <c r="BC43" s="11"/>
@@ -9068,7 +9068,7 @@
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
       <c r="R44" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S44" s="11"/>
       <c r="T44" s="11"/>
@@ -9103,11 +9103,11 @@
       <c r="AW44" s="11"/>
       <c r="AX44" s="8"/>
       <c r="AY44" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ44" s="11"/>
       <c r="BA44" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB44" s="11"/>
       <c r="BC44" s="11"/>
@@ -9147,7 +9147,7 @@
       <c r="P45" s="11"/>
       <c r="Q45" s="11"/>
       <c r="R45" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S45" s="11"/>
       <c r="T45" s="11"/>
@@ -9182,11 +9182,11 @@
       <c r="AW45" s="11"/>
       <c r="AX45" s="8"/>
       <c r="AY45" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ45" s="11"/>
       <c r="BA45" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB45" s="11"/>
       <c r="BC45" s="11"/>
@@ -9226,7 +9226,7 @@
       <c r="P46" s="11"/>
       <c r="Q46" s="11"/>
       <c r="R46" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S46" s="11"/>
       <c r="T46" s="11"/>
@@ -9261,11 +9261,11 @@
       <c r="AW46" s="11"/>
       <c r="AX46" s="8"/>
       <c r="AY46" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ46" s="11"/>
       <c r="BA46" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB46" s="11"/>
       <c r="BC46" s="11"/>
@@ -9305,7 +9305,7 @@
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
       <c r="R47" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S47" s="11"/>
       <c r="T47" s="11"/>
@@ -9340,11 +9340,11 @@
       <c r="AW47" s="11"/>
       <c r="AX47" s="8"/>
       <c r="AY47" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ47" s="11"/>
       <c r="BA47" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB47" s="11"/>
       <c r="BC47" s="11"/>
@@ -9384,7 +9384,7 @@
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
       <c r="R48" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S48" s="11"/>
       <c r="T48" s="11"/>
@@ -9419,11 +9419,11 @@
       <c r="AW48" s="11"/>
       <c r="AX48" s="8"/>
       <c r="AY48" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ48" s="11"/>
       <c r="BA48" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB48" s="11"/>
       <c r="BC48" s="11"/>
@@ -9463,7 +9463,7 @@
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
       <c r="R49" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S49" s="11"/>
       <c r="T49" s="11"/>
@@ -9498,11 +9498,11 @@
       <c r="AW49" s="11"/>
       <c r="AX49" s="8"/>
       <c r="AY49" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ49" s="11"/>
       <c r="BA49" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB49" s="11"/>
       <c r="BC49" s="11"/>
@@ -9542,7 +9542,7 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
       <c r="R50" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S50" s="11"/>
       <c r="T50" s="11"/>
@@ -9577,11 +9577,11 @@
       <c r="AW50" s="11"/>
       <c r="AX50" s="8"/>
       <c r="AY50" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ50" s="11"/>
       <c r="BA50" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB50" s="11"/>
       <c r="BC50" s="11"/>
@@ -9621,7 +9621,7 @@
       <c r="P51" s="11"/>
       <c r="Q51" s="11"/>
       <c r="R51" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S51" s="11"/>
       <c r="T51" s="11"/>
@@ -9656,11 +9656,11 @@
       <c r="AW51" s="11"/>
       <c r="AX51" s="8"/>
       <c r="AY51" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ51" s="11"/>
       <c r="BA51" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB51" s="11"/>
       <c r="BC51" s="11"/>
@@ -9700,7 +9700,7 @@
       <c r="P52" s="11"/>
       <c r="Q52" s="11"/>
       <c r="R52" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S52" s="11"/>
       <c r="T52" s="11"/>
@@ -9735,11 +9735,11 @@
       <c r="AW52" s="11"/>
       <c r="AX52" s="8"/>
       <c r="AY52" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ52" s="11"/>
       <c r="BA52" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB52" s="11"/>
       <c r="BC52" s="11"/>
@@ -9779,7 +9779,7 @@
       <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
       <c r="R53" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S53" s="11"/>
       <c r="T53" s="11"/>
@@ -9814,11 +9814,11 @@
       <c r="AW53" s="11"/>
       <c r="AX53" s="8"/>
       <c r="AY53" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ53" s="11"/>
       <c r="BA53" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB53" s="11"/>
       <c r="BC53" s="11"/>
@@ -9858,7 +9858,7 @@
       <c r="P54" s="11"/>
       <c r="Q54" s="11"/>
       <c r="R54" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S54" s="11"/>
       <c r="T54" s="11"/>
@@ -9893,11 +9893,11 @@
       <c r="AW54" s="11"/>
       <c r="AX54" s="8"/>
       <c r="AY54" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ54" s="11"/>
       <c r="BA54" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB54" s="11"/>
       <c r="BC54" s="11"/>
@@ -9937,7 +9937,7 @@
       <c r="P55" s="11"/>
       <c r="Q55" s="11"/>
       <c r="R55" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S55" s="11"/>
       <c r="T55" s="11"/>
@@ -9972,11 +9972,11 @@
       <c r="AW55" s="11"/>
       <c r="AX55" s="8"/>
       <c r="AY55" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ55" s="11"/>
       <c r="BA55" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB55" s="11"/>
       <c r="BC55" s="11"/>
@@ -10016,7 +10016,7 @@
       <c r="P56" s="11"/>
       <c r="Q56" s="11"/>
       <c r="R56" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S56" s="11"/>
       <c r="T56" s="11"/>
@@ -10051,11 +10051,11 @@
       <c r="AW56" s="11"/>
       <c r="AX56" s="8"/>
       <c r="AY56" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ56" s="11"/>
       <c r="BA56" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB56" s="11"/>
       <c r="BC56" s="11"/>
@@ -10095,7 +10095,7 @@
       <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
       <c r="R57" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S57" s="11"/>
       <c r="T57" s="11"/>
@@ -10130,11 +10130,11 @@
       <c r="AW57" s="11"/>
       <c r="AX57" s="8"/>
       <c r="AY57" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ57" s="11"/>
       <c r="BA57" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB57" s="11"/>
       <c r="BC57" s="11"/>
@@ -10174,7 +10174,7 @@
       <c r="P58" s="11"/>
       <c r="Q58" s="11"/>
       <c r="R58" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
@@ -10209,11 +10209,11 @@
       <c r="AW58" s="11"/>
       <c r="AX58" s="8"/>
       <c r="AY58" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ58" s="11"/>
       <c r="BA58" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB58" s="11"/>
       <c r="BC58" s="11"/>
@@ -10253,7 +10253,7 @@
       <c r="P59" s="11"/>
       <c r="Q59" s="11"/>
       <c r="R59" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S59" s="11"/>
       <c r="T59" s="11"/>
@@ -10288,11 +10288,11 @@
       <c r="AW59" s="11"/>
       <c r="AX59" s="8"/>
       <c r="AY59" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ59" s="11"/>
       <c r="BA59" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB59" s="11"/>
       <c r="BC59" s="11"/>
@@ -10332,7 +10332,7 @@
       <c r="P60" s="11"/>
       <c r="Q60" s="11"/>
       <c r="R60" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S60" s="11"/>
       <c r="T60" s="11"/>
@@ -10367,11 +10367,11 @@
       <c r="AW60" s="11"/>
       <c r="AX60" s="8"/>
       <c r="AY60" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ60" s="11"/>
       <c r="BA60" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB60" s="11"/>
       <c r="BC60" s="11"/>
@@ -10411,7 +10411,7 @@
       <c r="P61" s="11"/>
       <c r="Q61" s="11"/>
       <c r="R61" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S61" s="11"/>
       <c r="T61" s="11"/>
@@ -10446,11 +10446,11 @@
       <c r="AW61" s="11"/>
       <c r="AX61" s="8"/>
       <c r="AY61" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ61" s="11"/>
       <c r="BA61" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB61" s="11"/>
       <c r="BC61" s="11"/>
@@ -10490,7 +10490,7 @@
       <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
       <c r="R62" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S62" s="11"/>
       <c r="T62" s="11"/>
@@ -10525,11 +10525,11 @@
       <c r="AW62" s="11"/>
       <c r="AX62" s="8"/>
       <c r="AY62" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ62" s="11"/>
       <c r="BA62" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB62" s="11"/>
       <c r="BC62" s="11"/>
@@ -10569,7 +10569,7 @@
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
       <c r="R63" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S63" s="11"/>
       <c r="T63" s="11"/>
@@ -10604,11 +10604,11 @@
       <c r="AW63" s="11"/>
       <c r="AX63" s="8"/>
       <c r="AY63" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ63" s="11"/>
       <c r="BA63" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB63" s="11"/>
       <c r="BC63" s="11"/>
@@ -10648,7 +10648,7 @@
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
       <c r="R64" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S64" s="11"/>
       <c r="T64" s="11"/>
@@ -10683,11 +10683,11 @@
       <c r="AW64" s="11"/>
       <c r="AX64" s="8"/>
       <c r="AY64" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ64" s="11"/>
       <c r="BA64" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB64" s="11"/>
       <c r="BC64" s="11"/>
@@ -10727,7 +10727,7 @@
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
       <c r="R65" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S65" s="11"/>
       <c r="T65" s="11"/>
@@ -10762,11 +10762,11 @@
       <c r="AW65" s="11"/>
       <c r="AX65" s="8"/>
       <c r="AY65" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ65" s="11"/>
       <c r="BA65" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB65" s="11"/>
       <c r="BC65" s="11"/>
@@ -10806,7 +10806,7 @@
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
       <c r="R66" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S66" s="11"/>
       <c r="T66" s="11"/>
@@ -10841,11 +10841,11 @@
       <c r="AW66" s="11"/>
       <c r="AX66" s="8"/>
       <c r="AY66" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ66" s="11"/>
       <c r="BA66" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB66" s="11"/>
       <c r="BC66" s="11"/>
@@ -10885,7 +10885,7 @@
       <c r="P67" s="11"/>
       <c r="Q67" s="11"/>
       <c r="R67" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S67" s="11"/>
       <c r="T67" s="11"/>
@@ -10920,11 +10920,11 @@
       <c r="AW67" s="11"/>
       <c r="AX67" s="8"/>
       <c r="AY67" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ67" s="11"/>
       <c r="BA67" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB67" s="11"/>
       <c r="BC67" s="11"/>
@@ -10964,7 +10964,7 @@
       <c r="P68" s="11"/>
       <c r="Q68" s="11"/>
       <c r="R68" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="11"/>
@@ -10999,11 +10999,11 @@
       <c r="AW68" s="11"/>
       <c r="AX68" s="8"/>
       <c r="AY68" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ68" s="11"/>
       <c r="BA68" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB68" s="11"/>
       <c r="BC68" s="11"/>
@@ -11043,7 +11043,7 @@
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
       <c r="R69" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S69" s="11"/>
       <c r="T69" s="11"/>
@@ -11078,11 +11078,11 @@
       <c r="AW69" s="11"/>
       <c r="AX69" s="8"/>
       <c r="AY69" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ69" s="11"/>
       <c r="BA69" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB69" s="11"/>
       <c r="BC69" s="11"/>
@@ -11122,7 +11122,7 @@
       <c r="P70" s="11"/>
       <c r="Q70" s="11"/>
       <c r="R70" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S70" s="11"/>
       <c r="T70" s="11"/>
@@ -11157,11 +11157,11 @@
       <c r="AW70" s="11"/>
       <c r="AX70" s="8"/>
       <c r="AY70" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ70" s="11"/>
       <c r="BA70" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB70" s="11"/>
       <c r="BC70" s="11"/>
@@ -11201,7 +11201,7 @@
       <c r="P71" s="11"/>
       <c r="Q71" s="11"/>
       <c r="R71" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S71" s="11"/>
       <c r="T71" s="11"/>
@@ -11236,11 +11236,11 @@
       <c r="AW71" s="11"/>
       <c r="AX71" s="8"/>
       <c r="AY71" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ71" s="11"/>
       <c r="BA71" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB71" s="11"/>
       <c r="BC71" s="11"/>
@@ -11280,7 +11280,7 @@
       <c r="P72" s="11"/>
       <c r="Q72" s="11"/>
       <c r="R72" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S72" s="11"/>
       <c r="T72" s="11"/>
@@ -11315,11 +11315,11 @@
       <c r="AW72" s="11"/>
       <c r="AX72" s="8"/>
       <c r="AY72" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ72" s="11"/>
       <c r="BA72" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB72" s="11"/>
       <c r="BC72" s="11"/>
@@ -11359,7 +11359,7 @@
       <c r="P73" s="11"/>
       <c r="Q73" s="11"/>
       <c r="R73" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S73" s="11"/>
       <c r="T73" s="11"/>
@@ -11394,11 +11394,11 @@
       <c r="AW73" s="11"/>
       <c r="AX73" s="8"/>
       <c r="AY73" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ73" s="11"/>
       <c r="BA73" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB73" s="11"/>
       <c r="BC73" s="11"/>
@@ -11438,7 +11438,7 @@
       <c r="P74" s="11"/>
       <c r="Q74" s="11"/>
       <c r="R74" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S74" s="11"/>
       <c r="T74" s="11"/>
@@ -11473,11 +11473,11 @@
       <c r="AW74" s="11"/>
       <c r="AX74" s="8"/>
       <c r="AY74" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ74" s="11"/>
       <c r="BA74" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB74" s="11"/>
       <c r="BC74" s="11"/>
@@ -11517,7 +11517,7 @@
       <c r="P75" s="11"/>
       <c r="Q75" s="11"/>
       <c r="R75" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S75" s="11"/>
       <c r="T75" s="11"/>
@@ -11552,11 +11552,11 @@
       <c r="AW75" s="11"/>
       <c r="AX75" s="8"/>
       <c r="AY75" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ75" s="11"/>
       <c r="BA75" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB75" s="11"/>
       <c r="BC75" s="11"/>
@@ -11596,7 +11596,7 @@
       <c r="P76" s="11"/>
       <c r="Q76" s="11"/>
       <c r="R76" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S76" s="11"/>
       <c r="T76" s="11"/>
@@ -11631,11 +11631,11 @@
       <c r="AW76" s="11"/>
       <c r="AX76" s="8"/>
       <c r="AY76" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ76" s="11"/>
       <c r="BA76" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB76" s="11"/>
       <c r="BC76" s="11"/>
@@ -11675,7 +11675,7 @@
       <c r="P77" s="11"/>
       <c r="Q77" s="11"/>
       <c r="R77" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S77" s="11"/>
       <c r="T77" s="11"/>
@@ -11710,11 +11710,11 @@
       <c r="AW77" s="11"/>
       <c r="AX77" s="8"/>
       <c r="AY77" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ77" s="11"/>
       <c r="BA77" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB77" s="11"/>
       <c r="BC77" s="11"/>
@@ -11754,7 +11754,7 @@
       <c r="P78" s="11"/>
       <c r="Q78" s="11"/>
       <c r="R78" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S78" s="11"/>
       <c r="T78" s="11"/>
@@ -11789,11 +11789,11 @@
       <c r="AW78" s="11"/>
       <c r="AX78" s="8"/>
       <c r="AY78" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ78" s="11"/>
       <c r="BA78" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB78" s="11"/>
       <c r="BC78" s="11"/>
@@ -11833,7 +11833,7 @@
       <c r="P79" s="11"/>
       <c r="Q79" s="11"/>
       <c r="R79" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S79" s="11"/>
       <c r="T79" s="11"/>
@@ -11868,11 +11868,11 @@
       <c r="AW79" s="11"/>
       <c r="AX79" s="8"/>
       <c r="AY79" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ79" s="11"/>
       <c r="BA79" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB79" s="11"/>
       <c r="BC79" s="11"/>
@@ -11912,7 +11912,7 @@
       <c r="P80" s="11"/>
       <c r="Q80" s="11"/>
       <c r="R80" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S80" s="11"/>
       <c r="T80" s="11"/>
@@ -11947,11 +11947,11 @@
       <c r="AW80" s="11"/>
       <c r="AX80" s="8"/>
       <c r="AY80" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ80" s="11"/>
       <c r="BA80" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB80" s="11"/>
       <c r="BC80" s="11"/>
@@ -11991,7 +11991,7 @@
       <c r="P81" s="11"/>
       <c r="Q81" s="11"/>
       <c r="R81" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S81" s="11"/>
       <c r="T81" s="11"/>
@@ -12026,11 +12026,11 @@
       <c r="AW81" s="11"/>
       <c r="AX81" s="8"/>
       <c r="AY81" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ81" s="11"/>
       <c r="BA81" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB81" s="11"/>
       <c r="BC81" s="11"/>
@@ -12070,7 +12070,7 @@
       <c r="P82" s="11"/>
       <c r="Q82" s="11"/>
       <c r="R82" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S82" s="11"/>
       <c r="T82" s="11"/>
@@ -12105,11 +12105,11 @@
       <c r="AW82" s="11"/>
       <c r="AX82" s="8"/>
       <c r="AY82" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ82" s="11"/>
       <c r="BA82" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB82" s="11"/>
       <c r="BC82" s="11"/>
@@ -12149,7 +12149,7 @@
       <c r="P83" s="11"/>
       <c r="Q83" s="11"/>
       <c r="R83" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S83" s="11"/>
       <c r="T83" s="11"/>
@@ -12184,11 +12184,11 @@
       <c r="AW83" s="11"/>
       <c r="AX83" s="8"/>
       <c r="AY83" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ83" s="11"/>
       <c r="BA83" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB83" s="11"/>
       <c r="BC83" s="11"/>
@@ -12228,7 +12228,7 @@
       <c r="P84" s="11"/>
       <c r="Q84" s="11"/>
       <c r="R84" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S84" s="11"/>
       <c r="T84" s="11"/>
@@ -12263,11 +12263,11 @@
       <c r="AW84" s="11"/>
       <c r="AX84" s="8"/>
       <c r="AY84" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ84" s="11"/>
       <c r="BA84" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB84" s="11"/>
       <c r="BC84" s="11"/>
@@ -12307,7 +12307,7 @@
       <c r="P85" s="11"/>
       <c r="Q85" s="11"/>
       <c r="R85" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S85" s="11"/>
       <c r="T85" s="11"/>
@@ -12342,11 +12342,11 @@
       <c r="AW85" s="11"/>
       <c r="AX85" s="8"/>
       <c r="AY85" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ85" s="11"/>
       <c r="BA85" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB85" s="11"/>
       <c r="BC85" s="11"/>
@@ -12386,7 +12386,7 @@
       <c r="P86" s="11"/>
       <c r="Q86" s="11"/>
       <c r="R86" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S86" s="11"/>
       <c r="T86" s="11"/>
@@ -12421,11 +12421,11 @@
       <c r="AW86" s="11"/>
       <c r="AX86" s="8"/>
       <c r="AY86" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ86" s="11"/>
       <c r="BA86" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB86" s="11"/>
       <c r="BC86" s="11"/>
@@ -12465,7 +12465,7 @@
       <c r="P87" s="11"/>
       <c r="Q87" s="11"/>
       <c r="R87" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S87" s="11"/>
       <c r="T87" s="11"/>
@@ -12500,11 +12500,11 @@
       <c r="AW87" s="11"/>
       <c r="AX87" s="8"/>
       <c r="AY87" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ87" s="11"/>
       <c r="BA87" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB87" s="11"/>
       <c r="BC87" s="11"/>
@@ -12544,7 +12544,7 @@
       <c r="P88" s="11"/>
       <c r="Q88" s="11"/>
       <c r="R88" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S88" s="11"/>
       <c r="T88" s="11"/>
@@ -12579,11 +12579,11 @@
       <c r="AW88" s="11"/>
       <c r="AX88" s="8"/>
       <c r="AY88" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ88" s="11"/>
       <c r="BA88" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB88" s="11"/>
       <c r="BC88" s="11"/>
@@ -12623,7 +12623,7 @@
       <c r="P89" s="11"/>
       <c r="Q89" s="11"/>
       <c r="R89" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S89" s="11"/>
       <c r="T89" s="11"/>
@@ -12658,11 +12658,11 @@
       <c r="AW89" s="11"/>
       <c r="AX89" s="8"/>
       <c r="AY89" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ89" s="11"/>
       <c r="BA89" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB89" s="11"/>
       <c r="BC89" s="11"/>
@@ -12702,7 +12702,7 @@
       <c r="P90" s="11"/>
       <c r="Q90" s="11"/>
       <c r="R90" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S90" s="11"/>
       <c r="T90" s="11"/>
@@ -12737,11 +12737,11 @@
       <c r="AW90" s="11"/>
       <c r="AX90" s="8"/>
       <c r="AY90" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ90" s="11"/>
       <c r="BA90" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB90" s="11"/>
       <c r="BC90" s="11"/>
@@ -12781,7 +12781,7 @@
       <c r="P91" s="11"/>
       <c r="Q91" s="11"/>
       <c r="R91" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S91" s="11"/>
       <c r="T91" s="11"/>
@@ -12816,11 +12816,11 @@
       <c r="AW91" s="11"/>
       <c r="AX91" s="8"/>
       <c r="AY91" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ91" s="11"/>
       <c r="BA91" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB91" s="11"/>
       <c r="BC91" s="11"/>
@@ -12860,7 +12860,7 @@
       <c r="P92" s="11"/>
       <c r="Q92" s="11"/>
       <c r="R92" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S92" s="11"/>
       <c r="T92" s="11"/>
@@ -12895,11 +12895,11 @@
       <c r="AW92" s="11"/>
       <c r="AX92" s="8"/>
       <c r="AY92" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ92" s="11"/>
       <c r="BA92" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB92" s="11"/>
       <c r="BC92" s="11"/>
@@ -12939,7 +12939,7 @@
       <c r="P93" s="11"/>
       <c r="Q93" s="11"/>
       <c r="R93" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S93" s="11"/>
       <c r="T93" s="11"/>
@@ -12974,11 +12974,11 @@
       <c r="AW93" s="11"/>
       <c r="AX93" s="8"/>
       <c r="AY93" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ93" s="11"/>
       <c r="BA93" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB93" s="11"/>
       <c r="BC93" s="11"/>
@@ -13018,7 +13018,7 @@
       <c r="P94" s="11"/>
       <c r="Q94" s="11"/>
       <c r="R94" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S94" s="11"/>
       <c r="T94" s="11"/>
@@ -13053,11 +13053,11 @@
       <c r="AW94" s="11"/>
       <c r="AX94" s="8"/>
       <c r="AY94" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ94" s="11"/>
       <c r="BA94" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB94" s="11"/>
       <c r="BC94" s="11"/>
@@ -13097,7 +13097,7 @@
       <c r="P95" s="11"/>
       <c r="Q95" s="11"/>
       <c r="R95" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S95" s="11"/>
       <c r="T95" s="11"/>
@@ -13132,11 +13132,11 @@
       <c r="AW95" s="11"/>
       <c r="AX95" s="8"/>
       <c r="AY95" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ95" s="11"/>
       <c r="BA95" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB95" s="11"/>
       <c r="BC95" s="11"/>
@@ -13176,7 +13176,7 @@
       <c r="P96" s="11"/>
       <c r="Q96" s="11"/>
       <c r="R96" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S96" s="11"/>
       <c r="T96" s="11"/>
@@ -13211,11 +13211,11 @@
       <c r="AW96" s="11"/>
       <c r="AX96" s="8"/>
       <c r="AY96" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ96" s="11"/>
       <c r="BA96" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB96" s="11"/>
       <c r="BC96" s="11"/>
@@ -13255,7 +13255,7 @@
       <c r="P97" s="11"/>
       <c r="Q97" s="11"/>
       <c r="R97" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S97" s="11"/>
       <c r="T97" s="11"/>
@@ -13290,11 +13290,11 @@
       <c r="AW97" s="11"/>
       <c r="AX97" s="8"/>
       <c r="AY97" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ97" s="11"/>
       <c r="BA97" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB97" s="11"/>
       <c r="BC97" s="11"/>
@@ -13334,7 +13334,7 @@
       <c r="P98" s="11"/>
       <c r="Q98" s="11"/>
       <c r="R98" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S98" s="11"/>
       <c r="T98" s="11"/>
@@ -13369,11 +13369,11 @@
       <c r="AW98" s="11"/>
       <c r="AX98" s="8"/>
       <c r="AY98" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ98" s="11"/>
       <c r="BA98" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB98" s="11"/>
       <c r="BC98" s="11"/>
@@ -13413,7 +13413,7 @@
       <c r="P99" s="11"/>
       <c r="Q99" s="11"/>
       <c r="R99" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S99" s="11"/>
       <c r="T99" s="11"/>
@@ -13448,11 +13448,11 @@
       <c r="AW99" s="11"/>
       <c r="AX99" s="8"/>
       <c r="AY99" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ99" s="11"/>
       <c r="BA99" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB99" s="11"/>
       <c r="BC99" s="11"/>
@@ -13492,7 +13492,7 @@
       <c r="P100" s="11"/>
       <c r="Q100" s="11"/>
       <c r="R100" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S100" s="11"/>
       <c r="T100" s="11"/>
@@ -13527,11 +13527,11 @@
       <c r="AW100" s="11"/>
       <c r="AX100" s="8"/>
       <c r="AY100" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ100" s="11"/>
       <c r="BA100" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB100" s="11"/>
       <c r="BC100" s="11"/>
@@ -13571,7 +13571,7 @@
       <c r="P101" s="11"/>
       <c r="Q101" s="11"/>
       <c r="R101" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S101" s="11"/>
       <c r="T101" s="11"/>
@@ -13606,11 +13606,11 @@
       <c r="AW101" s="11"/>
       <c r="AX101" s="8"/>
       <c r="AY101" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ101" s="11"/>
       <c r="BA101" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB101" s="11"/>
       <c r="BC101" s="11"/>
@@ -13650,7 +13650,7 @@
       <c r="P102" s="11"/>
       <c r="Q102" s="11"/>
       <c r="R102" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S102" s="11"/>
       <c r="T102" s="11"/>
@@ -13685,11 +13685,11 @@
       <c r="AW102" s="11"/>
       <c r="AX102" s="8"/>
       <c r="AY102" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ102" s="11"/>
       <c r="BA102" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB102" s="11"/>
       <c r="BC102" s="11"/>
@@ -13729,7 +13729,7 @@
       <c r="P103" s="11"/>
       <c r="Q103" s="11"/>
       <c r="R103" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S103" s="11"/>
       <c r="T103" s="11"/>
@@ -13764,11 +13764,11 @@
       <c r="AW103" s="11"/>
       <c r="AX103" s="8"/>
       <c r="AY103" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ103" s="11"/>
       <c r="BA103" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB103" s="11"/>
       <c r="BC103" s="11"/>
@@ -13808,7 +13808,7 @@
       <c r="P104" s="11"/>
       <c r="Q104" s="11"/>
       <c r="R104" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S104" s="11"/>
       <c r="T104" s="11"/>
@@ -13843,11 +13843,11 @@
       <c r="AW104" s="11"/>
       <c r="AX104" s="8"/>
       <c r="AY104" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AZ104" s="11"/>
       <c r="BA104" s="8" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="BB104" s="11"/>
       <c r="BC104" s="11"/>
@@ -13871,6 +13871,7 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="17">
+    <mergeCell ref="AE2:AL2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="BO2:BS2"/>
@@ -13887,7 +13888,6 @@
     <mergeCell ref="T2:Y2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AE2:AL2"/>
   </mergeCells>
   <dataValidations count="25">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error de llenado" error="No debe de contener espacios ni caracteres especiales." promptTitle="Indicaciones" prompt="El formato debe ser XAXX010101000." sqref="H4:H104 X4:X104 AT4:AT104" xr:uid="{B98F17B9-63D0-482A-929E-F8CFD205118A}">
@@ -14018,10 +14018,10 @@
   <sheetData>
     <row r="2" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -14086,7 +14086,7 @@
         <v>800</v>
       </c>
       <c r="C3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -14137,7 +14137,7 @@
         <v>897</v>
       </c>
       <c r="AL3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AN3" t="s">
         <v>901</v>
@@ -14151,7 +14151,7 @@
         <v>801</v>
       </c>
       <c r="C4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -14202,7 +14202,7 @@
         <v>898</v>
       </c>
       <c r="AL4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="AN4" t="s">
         <v>902</v>
@@ -14213,7 +14213,7 @@
     </row>
     <row r="5" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -14266,7 +14266,7 @@
     </row>
     <row r="6" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
@@ -14310,7 +14310,7 @@
     </row>
     <row r="7" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
@@ -14354,7 +14354,7 @@
     </row>
     <row r="8" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -14392,7 +14392,7 @@
     </row>
     <row r="9" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -14427,7 +14427,7 @@
     </row>
     <row r="10" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -14462,7 +14462,7 @@
     </row>
     <row r="11" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E11" t="s">
         <v>59</v>
@@ -14497,7 +14497,7 @@
     </row>
     <row r="12" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E12" t="s">
         <v>65</v>
@@ -14529,7 +14529,7 @@
     </row>
     <row r="13" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E13" t="s">
         <v>71</v>
@@ -14561,7 +14561,7 @@
     </row>
     <row r="14" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E14" t="s">
         <v>77</v>

</xml_diff>